<commit_message>
Fix bug report text
</commit_message>
<xml_diff>
--- a/Swag-labs-bug-report.xlsx
+++ b/Swag-labs-bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XERO\XERO-automation-interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB7A70-3471-462A-A8E3-F1C2B0B863B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C77368B-A078-4DD2-BBB8-433A092D4269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="171" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,123 +399,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1. Login to the products page by entering valid username and password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2. Add "Sauce Labs Backpack" into the cart by clicking "ADD TO CART" button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. Click the shopping cart icon on the right corner. 
-4. Click the "CHECKOUT" button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-5. Type "Kane" into the "First Name" field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-6. Type "Zhang" into the "Second Name" field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-7. Click "CONTINUE" button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Unable to type text into "Last Name" field from the checkout page</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -606,6 +489,113 @@
   </si>
   <si>
     <t>Verify the hamberger menu functionality of Swag Labs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. Login to the products page by entering valid username and password.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Add "Sauce Labs Backpack" into the cart by clicking "ADD TO CART" button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Click the shopping cart icon on the right corner. 
+4. Click the "CHECKOUT" button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+5. Type "Kane" into the "First Name" field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+6. Type "Zhang" into the "Last Name" field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+7. Click "CONTINUE" button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1137,7 +1127,9 @@
   </sheetPr>
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1476,22 +1468,22 @@
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="I10" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>23</v>
@@ -1500,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
@@ -1572,13 +1564,13 @@
         <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="9" t="s">
@@ -1614,32 +1606,32 @@
     </row>
     <row r="13" spans="1:27" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>24</v>

</xml_diff>